<commit_message>
More drones and more batteris
</commit_message>
<xml_diff>
--- a/drone-energy-estimates.xlsx
+++ b/drone-energy-estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ups/src/sdu-uas/irc-2020-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8CE08C-7FC7-0A46-9B40-0082F5E555D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36691A36-6655-254E-90E2-1559E71C2307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12140" yWindow="4300" windowWidth="28040" windowHeight="17440" xr2:uid="{03E33AD7-FC22-F04B-8E76-51EC143E76A3}"/>
+    <workbookView xWindow="12740" yWindow="4180" windowWidth="28040" windowHeight="17440" xr2:uid="{03E33AD7-FC22-F04B-8E76-51EC143E76A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -278,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -308,6 +308,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +628,7 @@
   <dimension ref="B2:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -874,7 +877,8 @@
         <v>22</v>
       </c>
       <c r="C9" s="1">
-        <v>4500</v>
+        <f>4500*6</f>
+        <v>27000</v>
       </c>
       <c r="D9" s="2">
         <v>22.2</v>
@@ -887,22 +891,22 @@
       </c>
       <c r="G9" s="7">
         <f t="shared" si="0"/>
-        <v>359640</v>
+        <v>2157840</v>
       </c>
       <c r="H9" s="8">
         <f t="shared" si="1"/>
-        <v>287712</v>
+        <v>1726272</v>
       </c>
       <c r="I9" s="9">
         <f t="shared" si="2"/>
-        <v>137.00571428571428</v>
+        <v>822.03428571428572</v>
       </c>
       <c r="J9" s="1">
         <v>9100</v>
       </c>
       <c r="K9" s="10">
         <f t="shared" si="3"/>
-        <v>1.505557299843014E-2</v>
+        <v>9.0333437990580842E-2</v>
       </c>
     </row>
     <row r="10" spans="2:11">
@@ -910,7 +914,8 @@
         <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>5700</v>
+        <f>5700*6</f>
+        <v>34200</v>
       </c>
       <c r="D10" s="2">
         <v>22.8</v>
@@ -923,22 +928,22 @@
       </c>
       <c r="G10" s="8">
         <f t="shared" si="0"/>
-        <v>467856</v>
+        <v>2807136</v>
       </c>
       <c r="H10" s="8">
         <f t="shared" si="1"/>
-        <v>374284.80000000005</v>
+        <v>2245708.8000000003</v>
       </c>
       <c r="I10" s="17">
         <f t="shared" si="2"/>
-        <v>155.95200000000003</v>
+        <v>935.7120000000001</v>
       </c>
       <c r="J10" s="2">
         <v>9600</v>
       </c>
       <c r="K10" s="10">
         <f t="shared" si="3"/>
-        <v>1.6245000000000002E-2</v>
+        <v>9.7470000000000015E-2</v>
       </c>
     </row>
     <row r="11" spans="2:11">
@@ -978,17 +983,19 @@
       </c>
     </row>
     <row r="13" spans="2:11">
-      <c r="C13" t="s">
+      <c r="C13" s="23" t="s">
         <v>28</v>
       </c>
+      <c r="D13" s="23"/>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="23">
         <v>640</v>
       </c>
+      <c r="D14" s="23"/>
       <c r="E14">
         <v>110</v>
       </c>
@@ -1016,10 +1023,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:I2"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>